<commit_message>
Correct month display and the use of "
</commit_message>
<xml_diff>
--- a/CdS_Mastodon/lib/toots/xlsx/toots_CdS_7.xlsx
+++ b/CdS_Mastodon/lib/toots/xlsx/toots_CdS_7.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:29:30</t>
+          <t>14:13:40</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"J'ai reçu la lettre de Monsieur le conseiller Wilken, directeur en chef de la Bibliothèque royale de Berlin ..." à Wilken, 1839-10-27, https://constance-de-salm.de/archiv/#/document/8124 #onthisday</t>
+          <t>»J'ai reçu la lettre de Monsieur le conseiller Wilken, directeur en chef de la Bibliothèque royale de Berlin ...« à Wilken, 1839-10-27, https://constance-de-salm.de/archiv/#/document/8124 #onthisday</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,12 +495,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12:18:47</t>
+          <t>13:13:46</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Cher ami, j’ai reçu hier ta lettre du 26, tu m’y apprends la mort de Mosler, ou du moins qu’elle paraît certaine ; ..." à Salm-Reifferscheidt-Dyck, 1844-10-29, https://constance-de-salm.de/archiv/#/document/5352 #onthisday</t>
+          <t>»Cher ami, j’ai reçu hier ta lettre du 26, tu m’y apprends la mort de Mosler, ou du moins qu’elle paraît certaine ; ...« à Salm-Reifferscheidt-Dyck, 1844-10-29, https://constance-de-salm.de/archiv/#/document/5352 #onthisday</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -522,12 +522,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>19:38:26</t>
+          <t>14:09:34</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Je suis entourée d’apprêts de voyage, ma chère amie, je me mets en route dans peu de jours ..." à Leroy de Bacre, 1835-10-30, https://constance-de-salm.de/archiv/#/document/9659 #onthisday</t>
+          <t>»Je suis entourée d’apprêts de voyage, ma chère amie, je me mets en route dans peu de jours ...« à Leroy de Bacre, 1835-10-30, https://constance-de-salm.de/archiv/#/document/9659 #onthisday</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -544,17 +544,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2030-11-8</t>
+          <t>2030-11-08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>19:00:33</t>
+          <t>14:16:33</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"J‘ai reçu votre lettre, il y a déjà quelque temps, ma chère cousine ..." à Novakowsky, 1841-11-08, https://constance-de-salm.de/archiv/#/document/11261 #onthisday</t>
+          <t>»J‘ai reçu votre lettre, il y a déjà quelque temps, ma chère cousine ...« à Novakowsky, 1841-11-08, https://constance-de-salm.de/archiv/#/document/11261 #onthisday</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -576,12 +576,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>09:07:09</t>
+          <t>17:53:41</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Au moment où je venais de faire partir la lettre que je vous ai écrite hier Monsieur, on est venu me dire que l’extrait mortuaire en question devait être légalisé à l’ambassade prussienne ..." à Pailliet, 1841-11-10, https://constance-de-salm.de/archiv/#/document/11263 #onthisday</t>
+          <t>»Au moment où je venais de faire partir la lettre que je vous ai écrite hier Monsieur, on est venu me dire que l’extrait mortuaire en question devait être légalisé à l’ambassade prussienne ...« à Pailliet, 1841-11-10, https://constance-de-salm.de/archiv/#/document/11263 #onthisday</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -603,12 +603,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>09:21:56</t>
+          <t>13:13:03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"J’ai reçu votre aimable lettre, mon cher voisin, et quoique nous devions bientôt nous voir ..." à Ladoucette, 1841-11-12, https://constance-de-salm.de/archiv/#/document/11264 #onthisday</t>
+          <t>»J’ai reçu votre aimable lettre, mon cher voisin, et quoique nous devions bientôt nous voir ...« à Ladoucette, 1841-11-12, https://constance-de-salm.de/archiv/#/document/11264 #onthisday</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -630,12 +630,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10:21:15</t>
+          <t>09:51:33</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Il y a déjà quelque temps que j’ai reçu votre lettre, Monsieur, et je me reprocherais ..." à Depping, 1840-11-16, https://constance-de-salm.de/archiv/#/document/10028 #onthisday</t>
+          <t>»Il y a déjà quelque temps que j’ai reçu votre lettre, Monsieur, et je me reprocherais ...« à Depping, 1840-11-16, https://constance-de-salm.de/archiv/#/document/10028 #onthisday</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -657,12 +657,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>08:51:20</t>
+          <t>18:37:07</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"J’ai reçu hier ta lettre du 13 et du 14, cher ami, je t’aurais écrit la veille pour t’annoncer la mort de Mollevault ..." à Salm-Reifferscheidt-Dyck, 1844-11-17, https://constance-de-salm.de/archiv/#/document/5351 #onthisday</t>
+          <t>»J’ai reçu hier ta lettre du 13 et du 14, cher ami, je t’aurais écrit la veille pour t’annoncer la mort de Mollevault ...« à Salm-Reifferscheidt-Dyck, 1844-11-17, https://constance-de-salm.de/archiv/#/document/5351 #onthisday</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -684,12 +684,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11:58:43</t>
+          <t>11:42:56</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"J’ai reçu votre lettre il y a quelque temps, ma chère amie, elle m’a fait beaucoup de plaisir ; ..." à Naigeon, 1840-11-19, https://constance-de-salm.de/archiv/#/document/11176 #onthisday</t>
+          <t>»J’ai reçu votre lettre il y a quelque temps, ma chère amie, elle m’a fait beaucoup de plaisir ; ...« à Naigeon, 1840-11-19, https://constance-de-salm.de/archiv/#/document/11176 #onthisday</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -711,12 +711,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>19:11:43</t>
+          <t>11:48:06</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Tu dois être à Paris demain, mon cher Félix, par conséquant tu pourras recevoir cette lettre un ou deux jours après ..." à Francq, 1842-11-20, https://constance-de-salm.de/archiv/#/document/7483 #onthisday</t>
+          <t>»Tu dois être à Paris demain, mon cher Félix, par conséquant tu pourras recevoir cette lettre un ou deux jours après ...« à Francq, 1842-11-20, https://constance-de-salm.de/archiv/#/document/7483 #onthisday</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -738,12 +738,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18:03:08</t>
+          <t>19:27:00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"J’ai été si souffrante tous ces jours-ci, cher ami, que je n’ai pas eu le courage de t‘écrire, ni même de rien faire ..." à Salm-Reifferscheidt-Dyck, 1844-11-23, https://constance-de-salm.de/archiv/#/document/5350 #onthisday</t>
+          <t>»J’ai été si souffrante tous ces jours-ci, cher ami, que je n’ai pas eu le courage de t‘écrire, ni même de rien faire ...« à Salm-Reifferscheidt-Dyck, 1844-11-23, https://constance-de-salm.de/archiv/#/document/5350 #onthisday</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -765,12 +765,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:33:31</t>
+          <t>11:06:50</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"La lettre que j'ai reçue de vous il y a quelque temps, mon cher voisin, m'a fait grand plaisir ..." à Ladoucette, 1842-11-24, https://constance-de-salm.de/archiv/#/document/7486 #onthisday</t>
+          <t>»La lettre que j'ai reçue de vous il y a quelque temps, mon cher voisin, m'a fait grand plaisir ...« à Ladoucette, 1842-11-24, https://constance-de-salm.de/archiv/#/document/7486 #onthisday</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -792,12 +792,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11:43:48</t>
+          <t>15:23:18</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"J’ai reçu avant-hier, cher ami, ta bonne lettre du 22, elle m’a fait grand plaisir; car enfin que tu espérais avoir à peu près fini tes affaires dans 15 jours ..." à Salm-Reifferscheidt-Dyck, 1844-11-27, https://constance-de-salm.de/archiv/#/document/5349 #onthisday</t>
+          <t>»J’ai reçu avant-hier, cher ami, ta bonne lettre du 22, elle m’a fait grand plaisir; car enfin que tu espérais avoir à peu près fini tes affaires dans 15 jours ...« à Salm-Reifferscheidt-Dyck, 1844-11-27, https://constance-de-salm.de/archiv/#/document/5349 #onthisday</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -819,12 +819,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16:36:54</t>
+          <t>13:47:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Je reçois à l’instant, cher ami, la lettre dans laquelle tu m’annonces ce fait que ton départ aura lieu sinon le 5, au moins peu de jours après : jamais bonne nouvelle ne vint plus à propos ; ..." à Salm-Reifferscheidt-Dyck, 1844-11-30, https://constance-de-salm.de/archiv/#/document/5348 #onthisday</t>
+          <t>»Je reçois à l’instant, cher ami, la lettre dans laquelle tu m’annonces ce fait que ton départ aura lieu sinon le 5, au moins peu de jours après : jamais bonne nouvelle ne vint plus à propos ; ...« à Salm-Reifferscheidt-Dyck, 1844-11-30, https://constance-de-salm.de/archiv/#/document/5348 #onthisday</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -841,17 +841,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2030-12-6</t>
+          <t>2030-12-06</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>18:18:33</t>
+          <t>15:50:52</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Voici, Monsieur, la légende que vous avez eu la complaisance de m'envoyer ..." à Forster, 1838-12-06, https://constance-de-salm.de/archiv/#/document/7974 #onthisday</t>
+          <t>»Voici, Monsieur, la légende que vous avez eu la complaisance de m'envoyer ...« à Forster, 1838-12-06, https://constance-de-salm.de/archiv/#/document/7974 #onthisday</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -868,17 +868,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2031-1-14</t>
+          <t>2031-01-14</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>13:31:06</t>
+          <t>11:13:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"Je n’entends point parler de toi, mon cher Alexandre; ..." à Francq, 1841-01-14, https://constance-de-salm.de/archiv/#/document/8835 #onthisday</t>
+          <t>»Je n’entends point parler de toi, mon cher Alexandre; ...« à Francq, 1841-01-14, https://constance-de-salm.de/archiv/#/document/8835 #onthisday</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -895,17 +895,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2031-2-19</t>
+          <t>2031-02-19</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:41:40</t>
+          <t>10:30:30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Mon mari, qui est ici depuis quelques jours, Monsieur, avait désiré vous voir ..." à Zur Hosen, 1837-02-19, https://constance-de-salm.de/archiv/#/document/7725 #onthisday</t>
+          <t>»Mon mari, qui est ici depuis quelques jours, Monsieur, avait désiré vous voir ...« à Zur Hosen, 1837-02-19, https://constance-de-salm.de/archiv/#/document/7725 #onthisday</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -922,17 +922,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2031-3-2</t>
+          <t>2031-03-02</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15:08:18</t>
+          <t>12:57:26</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"Il y a bien longtemps que je ne vous ai vu, Monsieur ..." à Villenave, 1842-03-02, https://constance-de-salm.de/archiv/#/document/11277 #onthisday</t>
+          <t>»Il y a bien longtemps que je ne vous ai vu, Monsieur ...« à Villenave, 1842-03-02, https://constance-de-salm.de/archiv/#/document/11277 #onthisday</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -949,17 +949,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2031-3-12</t>
+          <t>2031-03-12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17:44:33</t>
+          <t>15:28:21</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Je n'ai pu dormir cette nuit, ma chère amie, j'ai été sans cesse agitée par la crainte que Félix ..." à Francq, 1844-03-12, https://constance-de-salm.de/archiv/#/document/7718 #onthisday</t>
+          <t>»Je n'ai pu dormir cette nuit, ma chère amie, j'ai été sans cesse agitée par la crainte que Félix ...« à Francq, 1844-03-12, https://constance-de-salm.de/archiv/#/document/7718 #onthisday</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -976,17 +976,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2031-3-20</t>
+          <t>2031-03-20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18:17:23</t>
+          <t>14:26:10</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Je m’empresse, Monsieur, de répondre à la lettre que vous venez de m’écrire ..." à N.N., 1827-03-20, https://constance-de-salm.de/archiv/#/document/9063 #onthisday</t>
+          <t>»Je m’empresse, Monsieur, de répondre à la lettre que vous venez de m’écrire ...« à N.N., 1827-03-20, https://constance-de-salm.de/archiv/#/document/9063 #onthisday</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1003,17 +1003,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2031-3-25</t>
+          <t>2031-03-25</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17:14:57</t>
+          <t>11:07:12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"Je n’entends point parler de vous, ma chère cousine, je ne sais ..." à François, 1842-03-25, https://constance-de-salm.de/archiv/#/document/10981 #onthisday</t>
+          <t>»Je n’entends point parler de vous, ma chère cousine, je ne sais ...« à François, 1842-03-25, https://constance-de-salm.de/archiv/#/document/10981 #onthisday</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1030,17 +1030,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2031-3-29</t>
+          <t>2031-03-29</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>08:09:51</t>
+          <t>10:22:55</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>"Je conçois bien, mon cher voisin, qu‘à votre retour cous allez être accablé de travaux pour la Chambre; ..." à Ladoucette, 1842-03-29, https://constance-de-salm.de/archiv/#/document/11250 #onthisday</t>
+          <t>»Je conçois bien, mon cher voisin, qu‘à votre retour cous allez être accablé de travaux pour la Chambre; ...« à Ladoucette, 1842-03-29, https://constance-de-salm.de/archiv/#/document/11250 #onthisday</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1057,17 +1057,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2031-3-30</t>
+          <t>2031-03-30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>13:40:16</t>
+          <t>15:56:44</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>"Mille remerciements, Madame, du cadeau que vous m'avez fait des oeuvres posthumes de votre cher et digne mari ..." à Thurot, 1837-03-30, https://constance-de-salm.de/archiv/#/document/7749 #onthisday</t>
+          <t>»Mille remerciements, Madame, du cadeau que vous m'avez fait des oeuvres posthumes de votre cher et digne mari ...« à Thurot, 1837-03-30, https://constance-de-salm.de/archiv/#/document/7749 #onthisday</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1084,17 +1084,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2031-4-2</t>
+          <t>2031-04-02</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>17:10:46</t>
+          <t>09:27:19</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"Je suis toujours bien souffrante, Monsieur; je ne sors pas encore ..." à Barbier, 1842-04-02, https://constance-de-salm.de/archiv/#/document/11251 #onthisday</t>
+          <t>»Je suis toujours bien souffrante, Monsieur; je ne sors pas encore ...« à Barbier, 1842-04-02, https://constance-de-salm.de/archiv/#/document/11251 #onthisday</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1111,17 +1111,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2031-4-8</t>
+          <t>2031-04-08</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>14:19:03</t>
+          <t>09:49:17</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"Cher ami, je reçois à l'instant une lettre pour toi ..." à Salm-Reifferscheidt-Dyck, 1845-04-08, https://constance-de-salm.de/archiv/#/document/6145 #onthisday</t>
+          <t>»Cher ami, je reçois à l'instant une lettre pour toi ...« à Salm-Reifferscheidt-Dyck, 1845-04-08, https://constance-de-salm.de/archiv/#/document/6145 #onthisday</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1138,17 +1138,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2031-4-13</t>
+          <t>2031-04-13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11:54:54</t>
+          <t>08:04:33</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"Il y a bien longtemps que je ne t’ai donné de mes nouvelles, cher frère ..." à Théis, 1841-04-13, https://constance-de-salm.de/archiv/#/document/10949 #onthisday</t>
+          <t>»Il y a bien longtemps que je ne t’ai donné de mes nouvelles, cher frère ...« à Théis, 1841-04-13, https://constance-de-salm.de/archiv/#/document/10949 #onthisday</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1165,17 +1165,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2031-4-17</t>
+          <t>2031-04-17</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14:34:27</t>
+          <t>16:14:45</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>"Je suis toujours fort souffrante; je n'entends point parler de mes chers voisins ..." à Sanson de Pongerville, 1840-04-17, https://constance-de-salm.de/archiv/#/document/8170 #onthisday</t>
+          <t>»Je suis toujours fort souffrante; je n'entends point parler de mes chers voisins ...« à Sanson de Pongerville, 1840-04-17, https://constance-de-salm.de/archiv/#/document/8170 #onthisday</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1192,17 +1192,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2031-4-20</t>
+          <t>2031-04-20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>08:21:51</t>
+          <t>09:34:07</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"Si Monsieur Boucharlat est à Paris, dans ce moment, je l’engage à venir me voir; ..." à Boucharlat, 1833-04-20, https://constance-de-salm.de/archiv/#/document/9522 #onthisday</t>
+          <t>»Si Monsieur Boucharlat est à Paris, dans ce moment, je l’engage à venir me voir; ...« à Boucharlat, 1833-04-20, https://constance-de-salm.de/archiv/#/document/9522 #onthisday</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1219,17 +1219,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2031-4-20</t>
+          <t>2031-04-20</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:43:52</t>
+          <t>11:31:49</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>"Je veux vous dire moi-même, Madame et chère voisine, ce que j’ai déjà chargé Mademoiselle Trostorff de vous écrire; ..." à Locquenghien, 1835-04-20, https://constance-de-salm.de/archiv/#/document/9595 #onthisday</t>
+          <t>»Je veux vous dire moi-même, Madame et chère voisine, ce que j’ai déjà chargé Mademoiselle Trostorff de vous écrire; ...« à Locquenghien, 1835-04-20, https://constance-de-salm.de/archiv/#/document/9595 #onthisday</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1246,17 +1246,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2031-5-16</t>
+          <t>2031-05-16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>19:08:00</t>
+          <t>15:23:40</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"Il m'a été bien impossible, mon cher voisin, de vous parler hier de la lecture qu'un de nos amis ..." à Ladoucette, 1840-05-16, https://constance-de-salm.de/archiv/#/document/8181 #onthisday</t>
+          <t>»Il m'a été bien impossible, mon cher voisin, de vous parler hier de la lecture qu'un de nos amis ...« à Ladoucette, 1840-05-16, https://constance-de-salm.de/archiv/#/document/8181 #onthisday</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1273,17 +1273,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2031-5-20</t>
+          <t>2031-05-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>15:41:32</t>
+          <t>10:30:07</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>"Je regrette fort, Monsieur et ancien ami, de n’avoir pu vous voir ainsi que Madame Ponce avant de partir ..." à Ponce, 1827-05-20, https://constance-de-salm.de/archiv/#/document/9079 #onthisday</t>
+          <t>»Je regrette fort, Monsieur et ancien ami, de n’avoir pu vous voir ainsi que Madame Ponce avant de partir ...« à Ponce, 1827-05-20, https://constance-de-salm.de/archiv/#/document/9079 #onthisday</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1300,17 +1300,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2031-5-20</t>
+          <t>2031-05-20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>18:21:10</t>
+          <t>15:16:51</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>"Je reçois à l’instant, Monsieur, une lettre de mon frère qui m’annonce que Monsieur Garot lui a fait une visite ..." à Pailliet, 1828-05-20, https://constance-de-salm.de/archiv/#/document/11351 #onthisday</t>
+          <t>»Je reçois à l’instant, Monsieur, une lettre de mon frère qui m’annonce que Monsieur Garot lui a fait une visite ...« à Pailliet, 1828-05-20, https://constance-de-salm.de/archiv/#/document/11351 #onthisday</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1327,17 +1327,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2031-5-27</t>
+          <t>2031-05-27</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>10:58:46</t>
+          <t>14:58:12</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"J'étais si entourée, et, en même temps, si occupée, lorsque je dictais les méchants petits vers ..." à Sanson de Pongerville, 1841-05-27, https://constance-de-salm.de/archiv/#/document/7422 #onthisday</t>
+          <t>»J'étais si entourée, et, en même temps, si occupée, lorsque je dictais les méchants petits vers ...« à Sanson de Pongerville, 1841-05-27, https://constance-de-salm.de/archiv/#/document/7422 #onthisday</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1354,17 +1354,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2031-5-28</t>
+          <t>2031-05-28</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>13:38:45</t>
+          <t>10:30:51</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"J'ai reçu, Monsieur, l'ouvrage que vous m'avez fait le plaisir de m'envoyer ..." à Roosmalen, 1840-05-28, https://constance-de-salm.de/archiv/#/document/8191 #onthisday</t>
+          <t>»J'ai reçu, Monsieur, l'ouvrage que vous m'avez fait le plaisir de m'envoyer ...« à Roosmalen, 1840-05-28, https://constance-de-salm.de/archiv/#/document/8191 #onthisday</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1381,17 +1381,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2031-5-29</t>
+          <t>2031-05-29</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>10:46:20</t>
+          <t>09:27:04</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"Je veux faire deux invitations à mon cher voisin, et à sa toute aimable famille ..." à Ladoucette, 1840-05-29, https://constance-de-salm.de/archiv/#/document/8194 #onthisday</t>
+          <t>»Je veux faire deux invitations à mon cher voisin, et à sa toute aimable famille ...« à Ladoucette, 1840-05-29, https://constance-de-salm.de/archiv/#/document/8194 #onthisday</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1408,17 +1408,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2031-6-1</t>
+          <t>2031-06-01</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>13:53:45</t>
+          <t>13:42:53</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>"Je m'empresse d'envoyer à Monsieur Paganel ma nouvelle épître qui a paru hier ..." à Paganel, 1831-06-01, https://constance-de-salm.de/archiv/#/document/6340 #onthisday</t>
+          <t>»Je m'empresse d'envoyer à Monsieur Paganel ma nouvelle épître qui a paru hier ...« à Paganel, 1831-06-01, https://constance-de-salm.de/archiv/#/document/6340 #onthisday</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1435,17 +1435,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2031-6-1</t>
+          <t>2031-06-01</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:25:57</t>
+          <t>15:27:40</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>"Il y a bien longtemps, Monsieur, que je n’ai reçu de vos nouvelles; je m’en inquiète; ..." à Boucharlat, 1832-06-01, https://constance-de-salm.de/archiv/#/document/9514 #onthisday</t>
+          <t>»Il y a bien longtemps, Monsieur, que je n’ai reçu de vos nouvelles; je m’en inquiète; ...« à Boucharlat, 1832-06-01, https://constance-de-salm.de/archiv/#/document/9514 #onthisday</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1462,17 +1462,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2031-6-3</t>
+          <t>2031-06-03</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>08:08:22</t>
+          <t>19:20:57</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>"Je regrette beaucoup, Monsieur, que vous soyez venu hier trop tard pour trouver encore mon frère chez moi ..." à Barbier, 1840-06-03, https://constance-de-salm.de/archiv/#/document/8196 #onthisday</t>
+          <t>»Je regrette beaucoup, Monsieur, que vous soyez venu hier trop tard pour trouver encore mon frère chez moi ...« à Barbier, 1840-06-03, https://constance-de-salm.de/archiv/#/document/8196 #onthisday</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1489,17 +1489,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2031-6-24</t>
+          <t>2031-06-24</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18:01:32</t>
+          <t>16:44:00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"Voici, Monsieur, ce que vient de me dire Monsieur Bignan qui retourne à l'instant à la campagne ..." à Villenave, 1841-06-24, https://constance-de-salm.de/archiv/#/document/7437 #onthisday</t>
+          <t>»Voici, Monsieur, ce que vient de me dire Monsieur Bignan qui retourne à l'instant à la campagne ...« à Villenave, 1841-06-24, https://constance-de-salm.de/archiv/#/document/7437 #onthisday</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1516,17 +1516,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2031-6-25</t>
+          <t>2031-06-25</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11:05:33</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"Monsieur Villenave vient de m'envoyer, Monsieur, le numéro du journal ..." à Christian, 1837-06-25, https://constance-de-salm.de/archiv/#/document/7787 #onthisday</t>
+          <t>»Monsieur Villenave vient de m'envoyer, Monsieur, le numéro du journal ...« à Christian, 1837-06-25, https://constance-de-salm.de/archiv/#/document/7787 #onthisday</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1543,17 +1543,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2031-6-29</t>
+          <t>2031-06-29</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>09:12:24</t>
+          <t>19:33:04</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"Vos vers sont charmants, mon cher voisin; j'avais du monde quand on me les a remis ..." à Ladoucette, 1841-06-29, https://constance-de-salm.de/archiv/#/document/7440 #onthisday</t>
+          <t>»Vos vers sont charmants, mon cher voisin; j'avais du monde quand on me les a remis ...« à Ladoucette, 1841-06-29, https://constance-de-salm.de/archiv/#/document/7440 #onthisday</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1570,17 +1570,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2031-7-12</t>
+          <t>2031-07-12</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>15:44:57</t>
+          <t>14:55:36</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>"Il y a bien longtemps, Monsieur, que je n’ai entendu parler de vous; ..." à Gohier, 1828-07-12, https://constance-de-salm.de/archiv/#/document/10480 #onthisday</t>
+          <t>»Il y a bien longtemps, Monsieur, que je n’ai entendu parler de vous; ...« à Gohier, 1828-07-12, https://constance-de-salm.de/archiv/#/document/10480 #onthisday</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1597,17 +1597,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2031-7-12</t>
+          <t>2031-07-12</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>10:56:07</t>
+          <t>15:29:09</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>"Il y a bien longtemps, Monsieur, que je n’ai entendu parler de vous; ..." à Gohier, 1828-07-12, https://constance-de-salm.de/archiv/#/document/9188 #onthisday</t>
+          <t>»Il y a bien longtemps, Monsieur, que je n’ai entendu parler de vous; ...« à Gohier, 1828-07-12, https://constance-de-salm.de/archiv/#/document/9188 #onthisday</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1624,17 +1624,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2031-7-20</t>
+          <t>2031-07-20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>09:48:52</t>
+          <t>17:46:51</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>"Monsieur Drais vient de m’envoyer, Madame, la lettre que vous lui avez écrite D ..." à Maleszewski, 1835-07-20, https://constance-de-salm.de/archiv/#/document/9627 #onthisday</t>
+          <t>»Monsieur Drais vient de m’envoyer, Madame, la lettre que vous lui avez écrite D ...« à Maleszewski, 1835-07-20, https://constance-de-salm.de/archiv/#/document/9627 #onthisday</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1651,17 +1651,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2031-7-20</t>
+          <t>2031-07-20</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>09:55:13</t>
+          <t>08:46:42</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>"Votre tout aimable billet que je viens de recevoir, Madame, m'a fait le plus grand plaisir ..." à Vien, 1838-07-20, https://constance-de-salm.de/archiv/#/document/7934 #onthisday</t>
+          <t>»Votre tout aimable billet que je viens de recevoir, Madame, m'a fait le plus grand plaisir ...« à Vien, 1838-07-20, https://constance-de-salm.de/archiv/#/document/7934 #onthisday</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1678,17 +1678,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2031-9-18</t>
+          <t>2031-09-18</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16:30:51</t>
+          <t>08:22:57</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"J'ai reçu, Monsieur, hier 17, votre lettre du 14, ce qui prouve qu'elle a été 3 jours en route ..." à Drais, 1839-09-18, https://constance-de-salm.de/archiv/#/document/8108 #onthisday</t>
+          <t>»J'ai reçu, Monsieur, hier 17, votre lettre du 14, ce qui prouve qu'elle a été 3 jours en route ...« à Drais, 1839-09-18, https://constance-de-salm.de/archiv/#/document/8108 #onthisday</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1710,12 +1710,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13:10:36</t>
+          <t>16:02:36</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"Cette lettre vous sera remise, Monsieur, par un de nos amis, Monsieur Jullien de Paris, auteur ..." à Ritz, 1842-10-30, https://constance-de-salm.de/archiv/#/document/7472 #onthisday</t>
+          <t>»Cette lettre vous sera remise, Monsieur, par un de nos amis, Monsieur Jullien de Paris, auteur ...« à Ritz, 1842-10-30, https://constance-de-salm.de/archiv/#/document/7472 #onthisday</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1732,17 +1732,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2032-3-30</t>
+          <t>2032-03-30</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>11:15:01</t>
+          <t>16:33:08</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>"C'est de ma vieille main rhumatisée, Monsieur, que je veux vous dire que je suis ici ..." à Berville, 1838-03-30, https://constance-de-salm.de/archiv/#/document/7896 #onthisday</t>
+          <t>»C'est de ma vieille main rhumatisée, Monsieur, que je veux vous dire que je suis ici ...« à Berville, 1838-03-30, https://constance-de-salm.de/archiv/#/document/7896 #onthisday</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1759,17 +1759,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2032-4-13</t>
+          <t>2032-04-13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>15:41:04</t>
+          <t>17:58:43</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>"Mes yeux me font tellement souffrir aujourd'hui, Monsieur ..." à Villenave, 1842-04-13, https://constance-de-salm.de/archiv/#/document/11253 #onthisday</t>
+          <t>»Mes yeux me font tellement souffrir aujourd'hui, Monsieur ...« à Villenave, 1842-04-13, https://constance-de-salm.de/archiv/#/document/11253 #onthisday</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1786,17 +1786,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2032-4-20</t>
+          <t>2032-04-20</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16:43:36</t>
+          <t>19:44:14</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"La campagne a été jusqu‘à présent si triste, Monsieur le colonel, et, en arrivant, j’ai été tellement accablée ..." à Schepeler, 1835-04-20, https://constance-de-salm.de/archiv/#/document/9596 #onthisday</t>
+          <t>»La campagne a été jusqu‘à présent si triste, Monsieur le colonel, et, en arrivant, j’ai été tellement accablée ...« à Schepeler, 1835-04-20, https://constance-de-salm.de/archiv/#/document/9596 #onthisday</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1813,17 +1813,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2032-4-20</t>
+          <t>2032-04-20</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10:44:27</t>
+          <t>13:29:11</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"Un de mes amis qui est venu chez moi, hier au soir, m’a dit, Monsieur, qu’il vous quittait ..." à Sauvo, 1836-04-20, https://constance-de-salm.de/archiv/#/document/9736 #onthisday</t>
+          <t>»Un de mes amis qui est venu chez moi, hier au soir, m’a dit, Monsieur, qu’il vous quittait ...« à Sauvo, 1836-04-20, https://constance-de-salm.de/archiv/#/document/9736 #onthisday</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1840,17 +1840,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2032-5-20</t>
+          <t>2032-05-20</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>12:11:56</t>
+          <t>12:11:37</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>"Cette lettre à laquelle j'ai voulu ajouter quelques mots, Monsieur ..." à Bavier, 1831-05-20, https://constance-de-salm.de/archiv/#/document/9502 #onthisday</t>
+          <t>»Cette lettre à laquelle j'ai voulu ajouter quelques mots, Monsieur ...« à Bavier, 1831-05-20, https://constance-de-salm.de/archiv/#/document/9502 #onthisday</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1867,17 +1867,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2032-5-20</t>
+          <t>2032-05-20</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:29:26</t>
+          <t>14:27:22</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>"Cette lettre à laquelle j'ai voulu ajouter quelques mots, Monsieur ..." à Bavier, 1831-05-20, https://constance-de-salm.de/archiv/#/document/6362 #onthisday</t>
+          <t>»Cette lettre à laquelle j'ai voulu ajouter quelques mots, Monsieur ...« à Bavier, 1831-05-20, https://constance-de-salm.de/archiv/#/document/6362 #onthisday</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1894,17 +1894,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2032-5-29</t>
+          <t>2032-05-29</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>12:35:41</t>
+          <t>13:43:58</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"Je m'empresse de répondre à la lettre que j'ai reçue de vous hier, Monsieur, et à laquelle était jointe le prospectus ..." à Forster, 1841-05-29, https://constance-de-salm.de/archiv/#/document/7425 #onthisday</t>
+          <t>»Je m'empresse de répondre à la lettre que j'ai reçue de vous hier, Monsieur, et à laquelle était jointe le prospectus ...« à Forster, 1841-05-29, https://constance-de-salm.de/archiv/#/document/7425 #onthisday</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1921,17 +1921,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2032-6-1</t>
+          <t>2032-06-01</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>13:32:24</t>
+          <t>19:02:26</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>"C'est encore moi; les affaires que j'ai à décider ce soir ..." à Ladoucette, 1837-06-01, https://constance-de-salm.de/archiv/#/document/7779 #onthisday</t>
+          <t>»C'est encore moi; les affaires que j'ai à décider ce soir ...« à Ladoucette, 1837-06-01, https://constance-de-salm.de/archiv/#/document/7779 #onthisday</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1948,17 +1948,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2032-6-25</t>
+          <t>2032-06-25</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:05:38</t>
+          <t>15:19:33</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>"Mille remerciements, Madame et amie, du bon ouvrage que vous m'avez fait le plaisir de m'envoyer ..." à Laya, 1840-06-25, https://constance-de-salm.de/archiv/#/document/8206 #onthisday</t>
+          <t>»Mille remerciements, Madame et amie, du bon ouvrage que vous m'avez fait le plaisir de m'envoyer ...« à Laya, 1840-06-25, https://constance-de-salm.de/archiv/#/document/8206 #onthisday</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1975,17 +1975,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2032-7-12</t>
+          <t>2032-07-12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>15:58:56</t>
+          <t>16:45:27</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>"Après avoir écrit ce matin à Monsieur et Madame Depping, j’ai craint d’avoir attaché trop d’importance ..." à Depping, 1833-07-12, https://constance-de-salm.de/archiv/#/document/9533 #onthisday</t>
+          <t>»Après avoir écrit ce matin à Monsieur et Madame Depping, j’ai craint d’avoir attaché trop d’importance ...« à Depping, 1833-07-12, https://constance-de-salm.de/archiv/#/document/9533 #onthisday</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2002,17 +2002,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2032-7-12</t>
+          <t>2032-07-12</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17:18:20</t>
+          <t>19:45:37</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"Je vous bombarde de recommandations, mon cher Duval, mais il va sans dire ..." à Duval, 1833-07-12, https://constance-de-salm.de/archiv/#/document/9534 #onthisday</t>
+          <t>»Je vous bombarde de recommandations, mon cher Duval, mais il va sans dire ...« à Duval, 1833-07-12, https://constance-de-salm.de/archiv/#/document/9534 #onthisday</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2029,17 +2029,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2032-7-20</t>
+          <t>2032-07-20</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>14:17:36</t>
+          <t>11:45:34</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>"Quand vous avez été parti hier, Monsieur, je me suis souvenue tout à coup des 4 vers que je vais vous dire ..." à Audiffret, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7450 #onthisday</t>
+          <t>»Quand vous avez été parti hier, Monsieur, je me suis souvenue tout à coup des 4 vers que je vais vous dire ...« à Audiffret, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7450 #onthisday</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2056,17 +2056,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2033-3-30</t>
+          <t>2033-03-30</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>12:29:47</t>
+          <t>09:46:46</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>"Si Monsieur et Madame de Pongerville sont libres jeudi à 7h, je les engage à venir ..." à Sanson de Pongerville, 1841-03-30, https://constance-de-salm.de/archiv/#/document/7220 #onthisday</t>
+          <t>»Si Monsieur et Madame de Pongerville sont libres jeudi à 7h, je les engage à venir ...« à Sanson de Pongerville, 1841-03-30, https://constance-de-salm.de/archiv/#/document/7220 #onthisday</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2083,17 +2083,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2033-4-20</t>
+          <t>2033-04-20</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>19:06:00</t>
+          <t>19:58:23</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"Le Prince m'a envoyé il y a déjà quelques temps, Monsieur, la lettre ..." à Sandt, 1838-04-20, https://constance-de-salm.de/archiv/#/document/7903 #onthisday</t>
+          <t>»Le Prince m'a envoyé il y a déjà quelques temps, Monsieur, la lettre ...« à Sandt, 1838-04-20, https://constance-de-salm.de/archiv/#/document/7903 #onthisday</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2110,17 +2110,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2033-5-20</t>
+          <t>2033-05-20</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>14:46:35</t>
+          <t>13:33:15</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"Il me semble, Monsieur, que je dois vous dire que j'ai renoncé à l'idée de faire paraître ..." à Bignan, 1840-05-20, https://constance-de-salm.de/archiv/#/document/8183 #onthisday</t>
+          <t>»Il me semble, Monsieur, que je dois vous dire que j'ai renoncé à l'idée de faire paraître ...« à Bignan, 1840-05-20, https://constance-de-salm.de/archiv/#/document/8183 #onthisday</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2137,17 +2137,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2033-5-20</t>
+          <t>2033-05-20</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:29:38</t>
+          <t>16:47:44</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>"Monsieur Boucharlat a dû vous engager de ma part, Monsieur et Madame, à venir dîner avec nous ..." à Mathon de Fogères, 1841-05-20, https://constance-de-salm.de/archiv/#/document/7414 #onthisday</t>
+          <t>»Monsieur Boucharlat a dû vous engager de ma part, Monsieur et Madame, à venir dîner avec nous ...« à Mathon de Fogères, 1841-05-20, https://constance-de-salm.de/archiv/#/document/7414 #onthisday</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2164,17 +2164,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2033-6-1</t>
+          <t>2033-06-01</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10:05:35</t>
+          <t>16:10:55</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>"Voici, mon cher voisin, l'itinéraire de ma journée en réponse de la vôtre ..." à Ladoucette, 1837-06-01, https://constance-de-salm.de/archiv/#/document/7778 #onthisday</t>
+          <t>»Voici, mon cher voisin, l'itinéraire de ma journée en réponse de la vôtre ...« à Ladoucette, 1837-06-01, https://constance-de-salm.de/archiv/#/document/7778 #onthisday</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2191,17 +2191,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2033-7-12</t>
+          <t>2033-07-12</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>19:20:50</t>
+          <t>18:01:11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"Je suis à la campagne depuis quelque temps, Monsieur, j’aurais été charmé de vous voir encore ..." à Tissot, 1836-07-12, https://constance-de-salm.de/archiv/#/document/9819 #onthisday</t>
+          <t>»Je suis à la campagne depuis quelque temps, Monsieur, j’aurais été charmé de vous voir encore ...« à Tissot, 1836-07-12, https://constance-de-salm.de/archiv/#/document/9819 #onthisday</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2218,17 +2218,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2033-7-20</t>
+          <t>2033-07-20</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10:30:19</t>
+          <t>15:44:57</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>"Mon très cher général, je m'ennuie fort de ne pas vous voir, je pensais que vous viendriez hier ..." à Saint-Mars, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7452 #onthisday</t>
+          <t>»Mon très cher général, je m'ennuie fort de ne pas vous voir, je pensais que vous viendriez hier ...« à Saint-Mars, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7452 #onthisday</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2245,17 +2245,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2034-4-20</t>
+          <t>2034-04-20</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11:28:13</t>
+          <t>14:15:38</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"Vous avez tant de choses à penser dans ce moment, Monsieur ..." à Sanson de Pongerville, 1842-04-20, https://constance-de-salm.de/archiv/#/document/11256 #onthisday</t>
+          <t>»Vous avez tant de choses à penser dans ce moment, Monsieur ...« à Sanson de Pongerville, 1842-04-20, https://constance-de-salm.de/archiv/#/document/11256 #onthisday</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2272,17 +2272,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2034-5-20</t>
+          <t>2034-05-20</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>12:19:01</t>
+          <t>08:03:39</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"Je suis accablée de visites ce matin, cher frère, il va m’en arriver d’autres ..." à Théis, 1842-05-20, https://constance-de-salm.de/archiv/#/document/10984 #onthisday</t>
+          <t>»Je suis accablée de visites ce matin, cher frère, il va m’en arriver d’autres ...« à Théis, 1842-05-20, https://constance-de-salm.de/archiv/#/document/10984 #onthisday</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2299,17 +2299,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2034-6-1</t>
+          <t>2034-06-01</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>17:00:51</t>
+          <t>08:58:42</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"La nuit porte conseil, Monsieur, comme je dois voir, ce matin, l'auteur de la „Nouvelle mode“, et que je pense bien ..." à Drais, 1841-06-01, https://constance-de-salm.de/archiv/#/document/7429 #onthisday</t>
+          <t>»La nuit porte conseil, Monsieur, comme je dois voir, ce matin, l'auteur de la „Nouvelle mode“, et que je pense bien ...« à Drais, 1841-06-01, https://constance-de-salm.de/archiv/#/document/7429 #onthisday</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2326,17 +2326,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2034-7-12</t>
+          <t>2034-07-12</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>13:38:03</t>
+          <t>10:17:30</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"Cher ami, je viens de faire envoyer à Hannen des billets d'une lotterie allemande ..." à Salm-Reifferscheidt-Dyck, 1844-07-12, https://constance-de-salm.de/archiv/#/document/5379 #onthisday</t>
+          <t>»Cher ami, je viens de faire envoyer à Hannen des billets d'une lotterie allemande ...« à Salm-Reifferscheidt-Dyck, 1844-07-12, https://constance-de-salm.de/archiv/#/document/5379 #onthisday</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2353,17 +2353,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2034-7-20</t>
+          <t>2034-07-20</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>17:52:21</t>
+          <t>12:27:34</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"Tu n'arrives pas, cher frère, comme tu le proposais si tu tardes encore tu ne viendras ici ..." à Théis, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7451 #onthisday</t>
+          <t>»Tu n'arrives pas, cher frère, comme tu le proposais si tu tardes encore tu ne viendras ici ...« à Théis, 1841-07-20, https://constance-de-salm.de/archiv/#/document/7451 #onthisday</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">

</xml_diff>